<commit_message>
new reference reports, start pictet prod
</commit_message>
<xml_diff>
--- a/data/AO_TPT_V5.0_Template.xlsx
+++ b/data/AO_TPT_V5.0_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugo Durand\Workspace\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugo Durand\Workspace\TPT_generator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040FAD02-C9F5-4168-A502-6BE0F9AD7A0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6754751-E444-4648-B1BF-00D6CDC5C438}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="663" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="663" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="363">
   <si>
     <t>Solvency II Reporting - Methodology</t>
   </si>
@@ -1354,9 +1354,6 @@
 - if dp54 = "K653*" then dp137="8"
 - if dp54 = "T" then dp137="11"
 - if dp54 &lt;&gt; "Kxxxx" or "T" then dp137="9"</t>
-  </si>
-  <si>
-    <t>BIL Invest - Absolute Return - I EUR CAP</t>
   </si>
   <si>
     <t>4_Portfolio currency (B)</t>
@@ -2732,7 +2729,7 @@
   </sheetPr>
   <dimension ref="A1:EK25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -2792,7 +2789,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E1" s="72" t="s">
         <v>11</v>
@@ -2846,19 +2843,19 @@
         <v>57</v>
       </c>
       <c r="V1" s="72" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="W1" s="72" t="s">
         <v>61</v>
       </c>
       <c r="X1" s="72" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="Y1" s="72" t="s">
         <v>65</v>
       </c>
       <c r="Z1" s="72" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AA1" s="72" t="s">
         <v>69</v>
@@ -2873,7 +2870,7 @@
         <v>75</v>
       </c>
       <c r="AE1" s="72" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AF1" s="72" t="s">
         <v>79</v>
@@ -2891,7 +2888,7 @@
         <v>87</v>
       </c>
       <c r="AK1" s="72" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AL1" s="72" t="s">
         <v>91</v>
@@ -2963,7 +2960,7 @@
         <v>134</v>
       </c>
       <c r="BI1" s="72" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BJ1" s="72" t="s">
         <v>138</v>
@@ -2975,7 +2972,7 @@
         <v>142</v>
       </c>
       <c r="BM1" s="72" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="BN1" s="72" t="s">
         <v>145</v>
@@ -2999,7 +2996,7 @@
         <v>157</v>
       </c>
       <c r="BU1" s="72" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="BV1" s="72" t="s">
         <v>161</v>
@@ -3158,7 +3155,7 @@
         <v>256</v>
       </c>
       <c r="DV1" s="72" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="DW1" s="72" t="s">
         <v>260</v>
@@ -3596,8 +3593,8 @@
   </sheetPr>
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -3624,9 +3621,7 @@
     </row>
     <row r="2" spans="1:11" ht="27.75">
       <c r="A2" s="13"/>
-      <c r="B2" s="14" t="s">
-        <v>353</v>
-      </c>
+      <c r="B2" s="14"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>

</xml_diff>